<commit_message>
Stretch water to cover area Update project timeline
</commit_message>
<xml_diff>
--- a/Project Breakdown by Blocker and Swimlane.xlsx
+++ b/Project Breakdown by Blocker and Swimlane.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Documents\Git Projects\GraphicsDX12\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\John\Documents\GraphicsDX12\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" xr2:uid="{30935AFF-951A-4E47-AC0A-A2E990CA66B8}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9045" xr2:uid="{30935AFF-951A-4E47-AC0A-A2E990CA66B8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Part1</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>Fill Group Assessment</t>
+  </si>
+  <si>
+    <t>Write a list of which object has which texture</t>
   </si>
 </sst>
 </file>
@@ -145,7 +148,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -173,8 +176,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="17">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -306,19 +315,6 @@
     </border>
     <border>
       <left style="medium">
-        <color theme="9"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
         <color theme="7"/>
       </left>
       <right style="thin">
@@ -381,6 +377,30 @@
       <top style="medium">
         <color theme="5" tint="-0.249977111117893"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color theme="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="9"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -391,14 +411,11 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -416,9 +433,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -428,12 +442,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -443,26 +451,57 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="12" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -780,136 +819,143 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7635F57E-D448-4F7C-9FE5-A5883A0B560C}">
-  <dimension ref="A1:K47"/>
+  <dimension ref="A1:L47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="8" width="16.5546875" customWidth="1"/>
-    <col min="9" max="9" width="15.6640625" customWidth="1"/>
-    <col min="10" max="10" width="20.44140625" customWidth="1"/>
+    <col min="1" max="9" width="16.5703125" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" customWidth="1"/>
+    <col min="11" max="11" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="27"/>
+      <c r="D1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="H1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-    </row>
-    <row r="2" spans="1:11" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="13" t="s">
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+    </row>
+    <row r="2" spans="1:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11" t="s">
+      <c r="B2" s="9"/>
+      <c r="C2" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="E2" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="F2" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="G2" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="I2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="23" t="s">
+      <c r="J2" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="J2" s="25" t="s">
+      <c r="K2" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="K2" s="1"/>
-    </row>
-    <row r="3" spans="1:11" s="5" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="14"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-    </row>
-    <row r="4" spans="1:11" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="10" t="s">
+      <c r="L2" s="1"/>
+    </row>
+    <row r="3" spans="1:12" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="29"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+    </row>
+    <row r="4" spans="1:12" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="3" t="s">
+      <c r="C4" s="28"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="20" t="s">
+      <c r="H4" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="12" t="s">
+      <c r="I4" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
-    </row>
-    <row r="5" spans="1:11" ht="87" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="18" t="s">
+      <c r="L4" s="1"/>
+    </row>
+    <row r="5" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+      <c r="A5" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="9" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="11"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="1"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="3"/>
       <c r="G5" s="1"/>
-      <c r="H5" s="22" t="s">
+      <c r="H5" s="1"/>
+      <c r="I5" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
-    </row>
-    <row r="6" spans="1:11" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="9"/>
-      <c r="B6" s="10" t="s">
+      <c r="L5" s="1"/>
+    </row>
+    <row r="6" spans="1:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="8"/>
+      <c r="B6" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="31"/>
+      <c r="D6" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -917,14 +963,15 @@
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
-    </row>
-    <row r="7" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="9"/>
-      <c r="B7" s="18" t="s">
+      <c r="L6" s="1"/>
+    </row>
+    <row r="7" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="8"/>
+      <c r="B7" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="1"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -932,8 +979,9 @@
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L7" s="1"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -945,8 +993,9 @@
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L8" s="1"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -958,8 +1007,9 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L9" s="1"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -971,8 +1021,9 @@
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L10" s="1"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -981,8 +1032,9 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -991,8 +1043,9 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1001,8 +1054,9 @@
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1011,8 +1065,9 @@
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1021,8 +1076,9 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1031,8 +1087,9 @@
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1041,8 +1098,9 @@
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1051,8 +1109,9 @@
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1061,8 +1120,9 @@
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I19" s="1"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1071,8 +1131,9 @@
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1081,8 +1142,9 @@
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1091,8 +1153,9 @@
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1101,8 +1164,9 @@
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I23" s="1"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1111,8 +1175,9 @@
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I24" s="1"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1121,8 +1186,9 @@
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I25" s="1"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1131,8 +1197,9 @@
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I26" s="1"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1141,8 +1208,9 @@
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I27" s="1"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1151,8 +1219,9 @@
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I28" s="1"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1161,8 +1230,9 @@
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I29" s="1"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1171,8 +1241,9 @@
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I30" s="1"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1181,8 +1252,9 @@
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I31" s="1"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -1191,8 +1263,9 @@
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I32" s="1"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -1201,8 +1274,9 @@
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I33" s="1"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -1211,8 +1285,9 @@
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I34" s="1"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -1221,8 +1296,9 @@
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I35" s="1"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -1231,8 +1307,9 @@
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I36" s="1"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -1241,8 +1318,9 @@
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I37" s="1"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -1251,8 +1329,9 @@
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I38" s="1"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -1261,8 +1340,9 @@
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I39" s="1"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -1271,8 +1351,9 @@
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I40" s="1"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -1281,8 +1362,9 @@
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I41" s="1"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -1291,8 +1373,9 @@
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I42" s="1"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -1301,8 +1384,9 @@
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I43" s="1"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -1311,8 +1395,9 @@
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I44" s="1"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -1321,8 +1406,9 @@
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I45" s="1"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -1331,8 +1417,9 @@
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I46" s="1"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -1341,6 +1428,7 @@
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
       <c r="H47" s="1"/>
+      <c r="I47" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>